<commit_message>
fix: Havia um erro na seleção da entidade entre cm e fpsm (estava invertido).
</commit_message>
<xml_diff>
--- a/tpl/dcasp v2024.01.99.xlsx
+++ b/tpl/dcasp v2024.01.99.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B417CF-5B0A-457D-A4CB-2ABE3342A4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E86850-66F6-4320-A101-AD15A8418039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4F7366A-F902-4471-8E3C-BFE20B26D311}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="13" activeTab="24" xr2:uid="{F4F7366A-F902-4471-8E3C-BFE20B26D311}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros Manuais" sheetId="1" r:id="rId1"/>
@@ -2818,7 +2818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2691581A-1C5D-436D-8A00-3D7C6FD59808}">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3174,7 +3174,7 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -3211,7 +3211,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -3562,7 +3563,7 @@
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C36" s="55"/>
       <c r="D36" s="55"/>
@@ -3601,6 +3602,7 @@
   <mergeCells count="1">
     <mergeCell ref="B36:D36"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4390,7 +4392,7 @@
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C78" s="55"/>
       <c r="D78" s="55"/>
@@ -4429,6 +4431,7 @@
   <mergeCells count="1">
     <mergeCell ref="B78:D78"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5395,7 +5398,7 @@
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
@@ -5434,6 +5437,7 @@
   <mergeCells count="1">
     <mergeCell ref="B95:D95"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5447,7 +5451,7 @@
   </sheetPr>
   <dimension ref="B2:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -6128,7 +6132,7 @@
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -6167,9 +6171,9 @@
   <mergeCells count="1">
     <mergeCell ref="B55:D55"/>
   </mergeCells>
-  <printOptions headings="1" gridLines="1"/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="62" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6181,7 +6185,7 @@
   </sheetPr>
   <dimension ref="B2:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -6761,7 +6765,7 @@
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -6800,6 +6804,7 @@
   <mergeCells count="1">
     <mergeCell ref="B55:D55"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7195,7 +7200,7 @@
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
@@ -7241,9 +7246,8 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="B10:B12"/>
   </mergeCells>
-  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7949,7 +7953,7 @@
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -7991,6 +7995,7 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B46:F46"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8004,7 +8009,7 @@
   </sheetPr>
   <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -8667,7 +8672,7 @@
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C38" s="55"/>
       <c r="D38" s="55"/>
@@ -9105,7 +9110,7 @@
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -9154,9 +9159,8 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
   </mergeCells>
-  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9185,7 +9189,7 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">"Fonte: MS Excel; Órgão emissor: "&amp;paramOrgaoEmissor&amp;"; Data de emissão: "&amp;TEXT(NOW(),"dd/mm/aaaa, \à\s hh:mm")</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -9548,7 +9552,7 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -10188,7 +10192,7 @@
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
@@ -10227,6 +10231,7 @@
   <mergeCells count="1">
     <mergeCell ref="B54:D54"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10512,7 +10517,7 @@
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
@@ -10551,6 +10556,7 @@
   <mergeCells count="1">
     <mergeCell ref="B28:D28"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11002,7 +11008,7 @@
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C40" s="55"/>
       <c r="D40" s="55"/>
@@ -11041,6 +11047,7 @@
   <mergeCells count="1">
     <mergeCell ref="B40:D40"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11167,7 +11174,7 @@
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
@@ -11206,6 +11213,7 @@
   <mergeCells count="1">
     <mergeCell ref="B15:D15"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11215,7 +11223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0FEF76-DC74-4C14-9D75-7EB72B9B44D2}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -12687,7 +12695,7 @@
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
@@ -12726,6 +12734,7 @@
   <mergeCells count="1">
     <mergeCell ref="B66:D66"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12916,7 +12925,7 @@
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C22" s="55"/>
       <c r="D22" s="55"/>
@@ -12955,7 +12964,8 @@
   <mergeCells count="1">
     <mergeCell ref="B22:D22"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -13176,7 +13186,7 @@
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -13215,7 +13225,8 @@
   <mergeCells count="1">
     <mergeCell ref="B24:D24"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -13228,7 +13239,7 @@
   </sheetPr>
   <dimension ref="B2:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
@@ -14687,7 +14698,7 @@
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C98" s="55"/>
       <c r="D98" s="55"/>
@@ -14729,8 +14740,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B97:C97"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="93" min="1" max="4" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
@@ -15201,7 +15216,7 @@
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 13/02/2025, às 15:44</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="23"/>
@@ -15238,7 +15253,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Corrigidos mais erros na geração das DCASPs.
</commit_message>
<xml_diff>
--- a/tpl/dcasp v2024.01.99.xlsx
+++ b/tpl/dcasp v2024.01.99.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E86850-66F6-4320-A101-AD15A8418039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0603F20-12FF-49D1-BDA8-34F2EDC59F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="13" activeTab="24" xr2:uid="{F4F7366A-F902-4471-8E3C-BFE20B26D311}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="13" activeTab="24" xr2:uid="{F4F7366A-F902-4471-8E3C-BFE20B26D311}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros Manuais" sheetId="1" r:id="rId1"/>
@@ -3174,7 +3174,7 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -3563,7 +3563,7 @@
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C36" s="55"/>
       <c r="D36" s="55"/>
@@ -4392,7 +4392,7 @@
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C78" s="55"/>
       <c r="D78" s="55"/>
@@ -5398,7 +5398,7 @@
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
@@ -6132,7 +6132,7 @@
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -6765,7 +6765,7 @@
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -7200,7 +7200,7 @@
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
@@ -7953,7 +7953,7 @@
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -8672,7 +8672,7 @@
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C38" s="55"/>
       <c r="D38" s="55"/>
@@ -9110,7 +9110,7 @@
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -9189,7 +9189,7 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">"Fonte: MS Excel; Órgão emissor: "&amp;paramOrgaoEmissor&amp;"; Data de emissão: "&amp;TEXT(NOW(),"dd/mm/aaaa, \à\s hh:mm")</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -9552,7 +9552,7 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -10192,7 +10192,7 @@
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
@@ -10517,7 +10517,7 @@
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
@@ -11008,7 +11008,7 @@
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C40" s="55"/>
       <c r="D40" s="55"/>
@@ -11174,7 +11174,7 @@
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
@@ -11224,7 +11224,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11273,11 +11273,11 @@
         <v>572</v>
       </c>
       <c r="B3" s="49" t="e">
-        <f>'BP Q0'!D14</f>
+        <f>'BP Q0'!D14+'BP Q0'!D16</f>
         <v>#REF!</v>
       </c>
       <c r="C3" s="49" t="e">
-        <f>'BF Q0A'!C49</f>
+        <f>'BF Q0A'!C49+'BF Q0A'!C50</f>
         <v>#REF!</v>
       </c>
       <c r="D3" s="49"/>
@@ -11291,11 +11291,11 @@
         <v>573</v>
       </c>
       <c r="B4" s="50" t="e">
-        <f>'BP Q0'!C14</f>
+        <f>'BP Q0'!C14+'BP Q0'!C16</f>
         <v>#REF!</v>
       </c>
       <c r="C4" s="50" t="e">
-        <f>'BF Q0B'!C49</f>
+        <f>'BF Q0B'!C49+'BF Q0B'!C50</f>
         <v>#REF!</v>
       </c>
       <c r="D4" s="50"/>
@@ -12695,7 +12695,7 @@
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
@@ -12925,7 +12925,7 @@
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C22" s="55"/>
       <c r="D22" s="55"/>
@@ -13186,7 +13186,7 @@
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
@@ -14698,7 +14698,7 @@
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="55" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C98" s="55"/>
       <c r="D98" s="55"/>
@@ -15216,7 +15216,7 @@
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="str">
         <f ca="1">paramFonte</f>
-        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 08:10</v>
+        <v>Fonte: MS Excel; Órgão emissor: Secretaria da Fazenda / Setor de Contabilidade; Data de emissão: 14/02/2025, às 11:07</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="23"/>

</xml_diff>